<commit_message>
add claim tst case
</commit_message>
<xml_diff>
--- a/src/testdata/LoginData.xlsx
+++ b/src/testdata/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nishikanta\OneDrive\Desktop\TestingFinalTraining\testng-automation\src\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40769F34-1110-4398-B142-8B60FBD04AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F0E16C-1371-4E0B-81B3-141C9704B1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1870" yWindow="3110" windowWidth="14400" windowHeight="8170" xr2:uid="{4FFDC96F-A004-4957-AFCE-E181194DED56}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>admin123</t>
-  </si>
-  <si>
-    <t>shjk</t>
   </si>
   <si>
     <t>Admin</t>
@@ -400,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17019DDD-F8B5-4300-815A-F92E83F5088E}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -421,18 +418,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>